<commit_message>
Added: Excel File uploaded for analysis
</commit_message>
<xml_diff>
--- a/Week_6_Data_Analysis/stock_tracker/uploaded_file.xlsx
+++ b/Week_6_Data_Analysis/stock_tracker/uploaded_file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve">Stock Name</t>
   </si>
@@ -37,55 +37,34 @@
     <t xml:space="preserve">Current Price</t>
   </si>
   <si>
-    <t xml:space="preserve">Apple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tesla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Google</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Amazon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microsoft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Intel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Walmart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spotify</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-04-03</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Square</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-09-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PayPal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-07-30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adobe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-08-17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lyft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2023-10-05</t>
+    <t xml:space="preserve">BHARTIARTL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HDFCBANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HINDUNILVR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICICIBANK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POLYCAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SBICARD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUNPHARMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TCS</t>
   </si>
 </sst>
 </file>
@@ -95,7 +74,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -178,8 +157,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -195,16 +178,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -396,233 +371,224 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="17.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.75"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>50</v>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>44941</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>150</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>170</v>
+      <c r="B2" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D2" s="5" t="n">
+        <v>1698.35</v>
+      </c>
+      <c r="E2" s="5" t="n">
+        <v>1800.8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>44967</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>700</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>750</v>
+      <c r="B3" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D3" s="5" t="n">
+        <v>1757.65</v>
+      </c>
+      <c r="E3" s="5" t="n">
+        <v>1869.6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="2" t="n">
-        <v>20</v>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>44990</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>2500</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>2600</v>
+      <c r="B4" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>2230.2</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>2365.2</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>1277.75</v>
+      </c>
+      <c r="E5" s="5" t="n">
+        <v>1347.9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="n">
-        <v>45036</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>3000</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="C6" s="3" t="n">
-        <v>45078</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>250</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="C6" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>402.5</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>421.65</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="C7" s="3" t="n">
-        <v>45082</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>50</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>2522.55</v>
+      </c>
+      <c r="E7" s="5" t="n">
+        <v>2678.3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>29</v>
-      </c>
-      <c r="C8" s="3" t="n">
-        <v>44998</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>654.5</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>580.5</v>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D8" s="5" t="n">
+        <v>4813.55</v>
+      </c>
+      <c r="E8" s="5" t="n">
+        <v>5227</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5" t="n">
-        <v>50</v>
-      </c>
-      <c r="C9" s="6" t="s">
+      <c r="B9" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>814</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>876</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="5" t="n">
-        <v>170.1</v>
-      </c>
-      <c r="E9" s="5" t="n">
-        <v>150.25</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>45751</v>
+      </c>
+      <c r="D10" s="5" t="n">
+        <v>1653.5</v>
+      </c>
+      <c r="E10" s="5" t="n">
+        <v>1706</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="5" t="n">
-        <v>15</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="5" t="n">
-        <v>200.5</v>
-      </c>
-      <c r="E10" s="5" t="n">
-        <v>220.35</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="5" t="n">
-        <v>30</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>17</v>
+      <c r="B11" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>45751</v>
       </c>
       <c r="D11" s="5" t="n">
-        <v>110.2</v>
+        <v>3178.3</v>
       </c>
       <c r="E11" s="5" t="n">
-        <v>100.75</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="5" t="n">
-        <v>10</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="5" t="n">
-        <v>450.85</v>
-      </c>
-      <c r="E12" s="5" t="n">
-        <v>460.4</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="5" t="n">
-        <v>60.75</v>
-      </c>
-      <c r="E13" s="5" t="n">
-        <v>50.5</v>
+        <v>3259.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>